<commit_message>
updated with api calls and new ui development
</commit_message>
<xml_diff>
--- a/amazon_data.xlsx
+++ b/amazon_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,266 +445,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Acer Aspire Lite AMD Ryzen 5 5500U Premium Thin and Light Laptop (16 GB RAM/512 GB SSD/Windows 11 Home) AL15-41, 39.62 cm (15.6") Full HD Display, Metal Body, Steel Gray, 1.59 KG</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>89,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Acer Aspire 5 Gaming Laptop 13th Gen Intel Core i5 (Windows 11 Home/ 16 GB RAM/ 512 GB SSD/NVIDIA GeForce RTX 2050), A515-58GM 39.62 cm (15.6") IPS Full HD Display, Steel Gray, 1.78 KG</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>80,490</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Acer Aspire 5 13th Gen Intel Core i3 (8 GB RAM/512 GB SSD/Windows 11 Home/MS Office), A515-58M 15.6" Full HD Display, Steel Gray, 1.75 KG</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>36,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Acer Aspire 5 Thin and Light Laptop 13th Gen Intel Core i3-1315U (8 GB RAM/512 GB SSD/Windows 11 Home/MS Office), A515-58P 15.6" Full HD Display, Steel Gray, Wi-Fi 6, 1.78 Kg</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>64,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Acer Aspire 5 Thin and Light Laptop 13th Gen Intel Core i3-1315U (Windows 11 Home/8 GB RAM/512 GB SSD) A515-58P 15.6" Full HD Display, Steel Gray, Wi-Fi 6, 1.78 KG</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>40,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Acer Aspire Lite 11th Gen Intel Core i3 Premium Metal Laptop (8GB RAM/512GB SSD/Windows 11 Home) AL15-51, 39.62cm (15.6") Full HD Display, Metal Body, Steel Gray, 1.59 Kg</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>40,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Acer Aspire 5 13th Gen Intel Core i5 (16 GB RAM/512 GB SSD/Windows 11 Home/MS Office), A515-58M 15.6" Full HD IPS 45% NTSC Display, Steel Gray, 1.75 KG</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>31,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Acer Aspire 5 Gaming Laptop 13th Gen Intel Core i5 (16 GB RAM/512 GB SSD/NVIDIA RTX 2050 4GB Graphics/Windows 11 Home), A515-58GM 15.6" Full HD Display, Steel Gray, 1.78 KG</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>54,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Acer Aspire 3 Laptop 13th Gen Intel Core i3-N305 Processor (Windows 11 Home/8 GB RAM/512 GB SSD/Intel UHD Graphics) A315-510P, 39.62 cm (15.6") Full HD Display, Pure Silver, 1.7 KG</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>57,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Acer Aspire 5 Gaming Laptop Intel Core i5 13th Gen (16 GB/512 GB SSD/Windows 11 Home/4 GB Graphics/NVIDIA GeForce RTX 2050) A514-56GM,14" WUXGA Display, 1.56 KG</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>59,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Microsoft New Surface Pro9 13" Intel 12 Gen i5 / 8GB / 128GB Platinum with Bluetooth,Wi-Fi, NFC Windows 11 Home, 365 Family 30-Day Trial &amp; Xbox Game Pass Ultimate 30-Day Trial</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>88,553</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Acer Aspire 3 (Intel Core i3 1215U Processor/ 8GB/ 512 GB SSD/Windows 11 Home/MS Office) A315-59 with 39.6 cm (15.6") Full HD Display /1.78kg</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>36,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Acer Aspire 5 Gaming Laptop 13th Gen Intel Core i5 (Windows 11 Home/ 8 GB RAM/ 512 GB SSD/NVIDIA GeForce RTX 2050), A515-58GM 39.62 cm (15.6") IPS Full HD Display, Steel Gray, 1.78 KG</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>62,499</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Acer Aspire 5 13th Gen Intel Core i5 (8 GB RAM/512 GB SSD/Windows 11 Home/MS Office), A514-56M 14" Full HD IPS 45% NTSC Display, Steel Gray, 1.4 KG</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>52,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Acer Aspire Lite 12th Gen Intel Core i3-1215U Premium Metal Laptop (Windows 11 Home/8 GB RAM/512GB SSD) AL15-52, 39.62cm (15.6") Full HD Display, Metal Body, Steel Gray, 1.59 Kg</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>34,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Acer Aspire Lite 11th Gen Intel Core i3 Premium Metal Laptop (8GB RAM/256GB SSD/Windows 11 Home) AL15-51, 39.62cm (15.6") Full HD Display, Metal Body, Steel Gray, 1.59 Kg</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>30,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Acer Aspire 5 Gaming Laptop Intel Core i7 13th Gen (8 GB/512 GB SSD/Windows 11 Home/4 GB Graphics/NVIDIA GeForce RTX 2050) A514-56GM,14" WUXGA Display, 1.56 KG</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>70,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Acer Aspire 5 Gaming Laptop Intel Core i5 13th Gen (8 GB/512 GB SSD/Windows 11 Home/4 GB Graphics/NVIDIA GeForce RTX 2050) A514-56GM,14" WUXGA Display, 1.56 KG</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>60,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Acer Aspire Lite 12th Gen Intel Core i5-1235U Thin and Light Laptop (Windows 11 Home/16GB RAM/512GB SSD/Intel Iris Xe Graphics) AL15-52, 39.62cm (15.6") Full HD Display, Metal Body, Steel Gray, 1.6 KG</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>38,689</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Acer Aspire 3 Intel Core i3 11th Gen- (8 GB/512 GB SSD/Windows 11 Home/MS Office/1.7 Kg/Silver) A315-58 with 15.6-inch (39.6 cms) Full HD Display Laptop</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>1,11,499</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Microsoft New Surface Pro9 13 Inch (33.03 cm) Intel Evo 12 Gen i5 / 8GB / 256GB Graphite with Windows 11 Home, Wi-Fi, 365 Family 30-Day Trial &amp; Xbox Game Pass Ultimate 30-Day Trial</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>1,08,990</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Microsoft New Surface Pro9 13" Intel evo 12 Gen i5 / 8GB / 256GB Forest with Windows 11 Home, 365 Family 30-Day Trial &amp; Xbox Game Pass Ultimate 30-Day Trial, Bluetooth</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>